<commit_message>
started writing to the output file
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AC075F2-9F1F-41A4-B6F7-9FAF5584512D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{7AC075F2-9F1F-41A4-B6F7-9FAF5584512D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FDE3EDE-90C9-4953-94A0-C30805E1E811}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A28934A-972A-4B86-9E4B-9B9EF184AD0A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="REPORT" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,6 +31,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>3. For the days selected in step two, identify all emails which denote a change detected. Open each email and ensure the details within (e.g. each change is captured within the monthly tracker (findings tab).</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,10 +387,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4602C9DE-E17E-477F-82EF-344C56581430}">
+  <dimension ref="A26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2576A46B-7317-4470-BDEF-7D6807DB2678}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
made progress in creating temp data table
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{7AC075F2-9F1F-41A4-B6F7-9FAF5584512D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FDE3EDE-90C9-4953-94A0-C30805E1E811}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{7AC075F2-9F1F-41A4-B6F7-9FAF5584512D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{577A1929-24B5-47AE-AF9D-CBFF0C205098}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A28934A-972A-4B86-9E4B-9B9EF184AD0A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>3. For the days selected in step two, identify all emails which denote a change detected. Open each email and ensure the details within (e.g. each change is captured within the monthly tracker (findings tab).</t>
+    <t>"3. For the days selected in step two, identify all emails which denote a change detected. Open each email and ensure the details within (e.g. each change is captured within the monthly tracker (findings tab)."</t>
   </si>
 </sst>
 </file>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4602C9DE-E17E-477F-82EF-344C56581430}">
   <dimension ref="A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:I26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
was able to output header and one selected date
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{7AC075F2-9F1F-41A4-B6F7-9FAF5584512D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99EED83C-91FE-4177-B2D4-13B0DA2E861B}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{7AC075F2-9F1F-41A4-B6F7-9FAF5584512D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE17CC1B-58C9-4F4B-97D8-17823A161612}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A28934A-972A-4B86-9E4B-9B9EF184AD0A}"/>
   </bookViews>
@@ -34,9 +34,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>"3. For the days selected in step two, identify all emails which denote a change detected. Open each email and ensure the details within (e.g. each change is captured within the monthly tracker (findings tab)."</t>
+  </si>
+  <si>
+    <t>testps9023</t>
+  </si>
+  <si>
+    <t>testps01</t>
+  </si>
+  <si>
+    <t>magic_qq_appl</t>
+  </si>
+  <si>
+    <t>testps0324</t>
+  </si>
+  <si>
+    <t>Selection 1 (Date)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Total Changes</t>
   </si>
 </sst>
 </file>
@@ -72,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,17 +410,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4602C9DE-E17E-477F-82EF-344C56581430}">
-  <dimension ref="A26"/>
+  <dimension ref="A26:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:H31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>43839</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D29" s="1"/>
+      <c r="H29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>